<commit_message>
rebuild functions: Search, Contracts List, Show PDF,
</commit_message>
<xml_diff>
--- a/РЕЕСТР Контракты.xlsx
+++ b/РЕЕСТР Контракты.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\!PROJ\PYTHON\Reestr_Contracts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\!PROJ\PYTHON\contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,9 @@
     <sheet name="Контракты (2)" sheetId="2" r:id="rId1"/>
     <sheet name="Контракты" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Контракты!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -6970,8 +6973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K528"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A511" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="J300" sqref="J300"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6989,7 +6993,7 @@
     <col min="11" max="11" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8176,7 +8180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>123</v>
       </c>
@@ -8496,7 +8500,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>151</v>
       </c>
@@ -11120,7 +11124,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>370</v>
       </c>
@@ -11152,7 +11156,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>373</v>
       </c>
@@ -11248,7 +11252,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>382</v>
       </c>
@@ -11280,7 +11284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="252" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>384</v>
       </c>
@@ -12176,7 +12180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="72" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>462</v>
       </c>
@@ -12560,7 +12564,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>487</v>
       </c>
@@ -12848,7 +12852,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>509</v>
       </c>
@@ -13264,7 +13268,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="48" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>547</v>
       </c>
@@ -13648,7 +13652,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="209" spans="1:10" ht="156" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" ht="144" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>575</v>
       </c>
@@ -14736,7 +14740,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="243" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>670</v>
       </c>
@@ -14960,7 +14964,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="250" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>689</v>
       </c>
@@ -15056,7 +15060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="253" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>696</v>
       </c>
@@ -15408,7 +15412,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>727</v>
       </c>
@@ -16080,7 +16084,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="48" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>780</v>
       </c>
@@ -16272,7 +16276,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>798</v>
       </c>
@@ -20240,7 +20244,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="415" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>1098</v>
       </c>
@@ -20464,7 +20468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="422" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>1116</v>
       </c>
@@ -20496,7 +20500,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="423" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>1119</v>
       </c>
@@ -20528,7 +20532,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="424" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
         <v>1121</v>
       </c>
@@ -20592,7 +20596,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="426" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
         <v>1116</v>
       </c>
@@ -20624,7 +20628,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="427" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>1132</v>
       </c>
@@ -20656,7 +20660,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="428" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
         <v>1119</v>
       </c>
@@ -20688,7 +20692,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="429" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>1121</v>
       </c>
@@ -20976,7 +20980,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="438" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
         <v>1161</v>
       </c>
@@ -21232,7 +21236,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="446" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
         <v>1184</v>
       </c>
@@ -21360,7 +21364,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="450" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A450" s="2" t="s">
         <v>1194</v>
       </c>
@@ -21744,7 +21748,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="462" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>1223</v>
       </c>
@@ -21872,7 +21876,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="466" spans="1:10" ht="264" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10" ht="252" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>1231</v>
       </c>
@@ -22256,7 +22260,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="478" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A478" s="2" t="s">
         <v>1258</v>
       </c>
@@ -22448,7 +22452,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="484" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A484" s="2" t="s">
         <v>1273</v>
       </c>
@@ -22480,7 +22484,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="485" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
         <v>1277</v>
       </c>
@@ -22576,7 +22580,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="488" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A488" s="2" t="s">
         <v>1285</v>
       </c>
@@ -22640,7 +22644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="490" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:10" ht="108" x14ac:dyDescent="0.25">
       <c r="A490" s="2" t="s">
         <v>1290</v>
       </c>
@@ -22704,7 +22708,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="492" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A492" s="2" t="s">
         <v>1273</v>
       </c>
@@ -22736,7 +22740,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="493" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
         <v>1297</v>
       </c>
@@ -22864,7 +22868,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="497" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:10" ht="108" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
         <v>1306</v>
       </c>
@@ -23056,7 +23060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="503" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:10" ht="108" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
         <v>1321</v>
       </c>
@@ -23248,7 +23252,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="509" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:10" ht="108" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
         <v>1333</v>
       </c>
@@ -23280,7 +23284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="510" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A510" s="2" t="s">
         <v>1335</v>
       </c>
@@ -23312,7 +23316,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="511" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
         <v>1337</v>
       </c>
@@ -23344,7 +23348,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="512" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A512" s="2" t="s">
         <v>1340</v>
       </c>
@@ -23472,7 +23476,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="516" spans="1:10" ht="108" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:10" ht="96" x14ac:dyDescent="0.25">
       <c r="A516" s="2" t="s">
         <v>1354</v>
       </c>
@@ -23504,7 +23508,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="517" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
         <v>1358</v>
       </c>
@@ -23760,7 +23764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="525" spans="1:10" ht="156" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:10" ht="144" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
         <v>1384</v>
       </c>

</xml_diff>